<commit_message>
Update to v4.6: Fix search/replace discrepancy and support long file paths
- v4.5: Fix issue where Save failure caused changes to be discarded (added Status/Message to report)

- v4.6: Support Windows extended-length paths (\\?\ prefix) to fix Save errors on deep paths

- Added README.md and updated Implementation Plan
</commit_message>
<xml_diff>
--- a/03.test/01_成果物(20250926納品分)/F4001_データストア一覧/F4001_DA_データストア一覧.xlsx
+++ b/03.test/01_成果物(20250926納品分)/F4001_データストア一覧/F4001_DA_データストア一覧.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
+  <workbookPr codeName="ThisWorkbook" checkCompatibility="true"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svn\202501_finance_system\doc\20_外部設計\01_成果物\F4001_データストア一覧\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A59B70-2BCA-4E50-BE10-63412642424C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="809"/>
   </bookViews>
   <sheets>
     <sheet name="変更履歴" sheetId="13" r:id="rId1"/>
@@ -27,40 +26,40 @@
     <sheet name="12.共通" sheetId="28" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'10.他システム連動'!$A$7:$BJ$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'11.マスタ管理'!$A$7:$BJ$139</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'12.共通'!$A$7:$BJ$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2.財務会計'!$A$7:$BJ$40</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'3.管理会計'!$A$7:$BJ$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'4.税務'!$A$7:$BJ$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'5.債権管理'!$A$7:$BJ$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'6.債務管理'!$A$7:$BJ$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'7.棚卸資産管理'!$A$7:$BJ$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'8.部門提供'!$A$7:$BJ$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'9.共計'!$A$7:$BJ$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'11.マスタ管理'!$A$1:$BJ$148</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="11">'12.共通'!$A$1:$BJ$50</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'2.財務会計'!$A$1:$BJ$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'3.管理会計'!$A$1:$BJ$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'4.税務'!$A$1:$BJ$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'5.債権管理'!$A$1:$BJ$52</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'6.債務管理'!$A$1:$BJ$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'7.棚卸資産管理'!$A$1:$BJ$58</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'8.部門提供'!$A$1:$BJ$56</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'9.共計'!$A$1:$BJ$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">変更履歴!$A$1:$BJ$60</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="9">'10.他システム連動'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="10">'11.マスタ管理'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="11">'12.共通'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'2.財務会計'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'3.管理会計'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'4.税務'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="4">'5.債権管理'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="5">'6.債務管理'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="6">'7.棚卸資産管理'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">'8.部門提供'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">'9.共計'!$1:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">変更履歴!$1:$5</definedName>
+    <definedName hidden="true" localSheetId="9" name="_xlnm._FilterDatabase">'10.他システム連動'!$A$7:$BJ$88</definedName>
+    <definedName hidden="true" localSheetId="10" name="_xlnm._FilterDatabase">'11.マスタ管理'!$A$7:$BJ$139</definedName>
+    <definedName hidden="true" localSheetId="11" name="_xlnm._FilterDatabase">'12.共通'!$A$7:$BJ$47</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">'2.財務会計'!$A$7:$BJ$40</definedName>
+    <definedName hidden="true" localSheetId="2" name="_xlnm._FilterDatabase">'3.管理会計'!$A$7:$BJ$39</definedName>
+    <definedName hidden="true" localSheetId="3" name="_xlnm._FilterDatabase">'4.税務'!$A$7:$BJ$14</definedName>
+    <definedName hidden="true" localSheetId="4" name="_xlnm._FilterDatabase">'5.債権管理'!$A$7:$BJ$50</definedName>
+    <definedName hidden="true" localSheetId="5" name="_xlnm._FilterDatabase">'6.債務管理'!$A$7:$BJ$46</definedName>
+    <definedName hidden="true" localSheetId="6" name="_xlnm._FilterDatabase">'7.棚卸資産管理'!$A$7:$BJ$55</definedName>
+    <definedName hidden="true" localSheetId="7" name="_xlnm._FilterDatabase">'8.部門提供'!$A$7:$BJ$53</definedName>
+    <definedName hidden="true" localSheetId="8" name="_xlnm._FilterDatabase">'9.共計'!$A$7:$BJ$37</definedName>
+    <definedName localSheetId="10" name="_xlnm.Print_Area">'11.マスタ管理'!$A$1:$BJ$148</definedName>
+    <definedName localSheetId="11" name="_xlnm.Print_Area">'12.共通'!$A$1:$BJ$50</definedName>
+    <definedName localSheetId="1" name="_xlnm.Print_Area">'2.財務会計'!$A$1:$BJ$44</definedName>
+    <definedName localSheetId="2" name="_xlnm.Print_Area">'3.管理会計'!$A$1:$BJ$43</definedName>
+    <definedName localSheetId="3" name="_xlnm.Print_Area">'4.税務'!$A$1:$BJ$33</definedName>
+    <definedName localSheetId="4" name="_xlnm.Print_Area">'5.債権管理'!$A$1:$BJ$52</definedName>
+    <definedName localSheetId="5" name="_xlnm.Print_Area">'6.債務管理'!$A$1:$BJ$49</definedName>
+    <definedName localSheetId="6" name="_xlnm.Print_Area">'7.棚卸資産管理'!$A$1:$BJ$58</definedName>
+    <definedName localSheetId="7" name="_xlnm.Print_Area">'8.部門提供'!$A$1:$BJ$56</definedName>
+    <definedName localSheetId="8" name="_xlnm.Print_Area">'9.共計'!$A$1:$BJ$42</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Area">変更履歴!$A$1:$BJ$60</definedName>
+    <definedName localSheetId="9" name="_xlnm.Print_Titles">'10.他システム連動'!$1:$7</definedName>
+    <definedName localSheetId="10" name="_xlnm.Print_Titles">'11.マスタ管理'!$1:$7</definedName>
+    <definedName localSheetId="11" name="_xlnm.Print_Titles">'12.共通'!$1:$7</definedName>
+    <definedName localSheetId="1" name="_xlnm.Print_Titles">'2.財務会計'!$1:$7</definedName>
+    <definedName localSheetId="2" name="_xlnm.Print_Titles">'3.管理会計'!$1:$7</definedName>
+    <definedName localSheetId="3" name="_xlnm.Print_Titles">'4.税務'!$1:$7</definedName>
+    <definedName localSheetId="4" name="_xlnm.Print_Titles">'5.債権管理'!$1:$7</definedName>
+    <definedName localSheetId="5" name="_xlnm.Print_Titles">'6.債務管理'!$1:$7</definedName>
+    <definedName localSheetId="6" name="_xlnm.Print_Titles">'7.棚卸資産管理'!$1:$7</definedName>
+    <definedName localSheetId="7" name="_xlnm.Print_Titles">'8.部門提供'!$1:$7</definedName>
+    <definedName localSheetId="8" name="_xlnm.Print_Titles">'9.共計'!$1:$7</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Titles">変更履歴!$1:$5</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -7835,8 +7834,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="ＭＳ Ｐ明朝"/>
@@ -7862,7 +7861,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="14"/>
       <name val="ＭＳ 明朝"/>
       <family val="1"/>
@@ -7887,7 +7886,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -7895,7 +7894,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <u/>
       <sz val="9"/>
       <color indexed="81"/>
@@ -7904,7 +7903,7 @@
       <charset val="128"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="MS P ゴシック"/>
@@ -7929,6 +7928,13 @@
       <name val="ＭＳ 明朝"/>
       <family val="1"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color rgb="FF4180C4"/>
+      <name val="ＭＳ Ｐ明朝"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -8495,471 +8501,474 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="22" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" quotePrefix="true" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="false">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{B10EBE38-8611-4439-81B3-FBBDC04B2242}"/>
-    <cellStyle name="標準 5" xfId="2" xr:uid="{6EE46151-8420-4F48-BD0C-92A8F5334001}"/>
+    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="標準 5" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8972,120 +8981,120 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
+<theme xmlns="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office テーマ">
+  <themeElements>
+    <clrScheme name="Office">
+      <dk1>
+        <sysClr val="windowText" lastClr="000000"/>
+      </dk1>
+      <lt1>
+        <sysClr val="window" lastClr="FFFFFF"/>
+      </lt1>
+      <dk2>
+        <srgbClr val="44546A"/>
+      </dk2>
+      <lt2>
+        <srgbClr val="E7E6E6"/>
+      </lt2>
+      <accent1>
+        <srgbClr val="5B9BD5"/>
+      </accent1>
+      <accent2>
+        <srgbClr val="ED7D31"/>
+      </accent2>
+      <accent3>
+        <srgbClr val="A5A5A5"/>
+      </accent3>
+      <accent4>
+        <srgbClr val="FFC000"/>
+      </accent4>
+      <accent5>
+        <srgbClr val="4472C4"/>
+      </accent5>
+      <accent6>
+        <srgbClr val="70AD47"/>
+      </accent6>
+      <hlink>
+        <srgbClr val="0563C1"/>
+      </hlink>
+      <folHlink>
+        <srgbClr val="954F72"/>
+      </folHlink>
+    </clrScheme>
+    <fontScheme name="Office">
+      <majorFont>
+        <latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="宋体"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Times New Roman"/>
+        <font script="Hebr" typeface="Times New Roman"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="MoolBoran"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Times New Roman"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </majorFont>
+      <minorFont>
+        <latin typeface="Calibri" panose="020F0502020204030204"/>
+        <ea typeface=""/>
+        <cs typeface=""/>
+        <font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <font script="Hang" typeface="맑은 고딕"/>
+        <font script="Hans" typeface="宋体"/>
+        <font script="Hant" typeface="新細明體"/>
+        <font script="Arab" typeface="Arial"/>
+        <font script="Hebr" typeface="Arial"/>
+        <font script="Thai" typeface="Tahoma"/>
+        <font script="Ethi" typeface="Nyala"/>
+        <font script="Beng" typeface="Vrinda"/>
+        <font script="Gujr" typeface="Shruti"/>
+        <font script="Khmr" typeface="DaunPenh"/>
+        <font script="Knda" typeface="Tunga"/>
+        <font script="Guru" typeface="Raavi"/>
+        <font script="Cans" typeface="Euphemia"/>
+        <font script="Cher" typeface="Plantagenet Cherokee"/>
+        <font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <font script="Tibt" typeface="Microsoft Himalaya"/>
+        <font script="Thaa" typeface="MV Boli"/>
+        <font script="Deva" typeface="Mangal"/>
+        <font script="Telu" typeface="Gautami"/>
+        <font script="Taml" typeface="Latha"/>
+        <font script="Syrc" typeface="Estrangelo Edessa"/>
+        <font script="Orya" typeface="Kalinga"/>
+        <font script="Mlym" typeface="Kartika"/>
+        <font script="Laoo" typeface="DokChampa"/>
+        <font script="Sinh" typeface="Iskoola Pota"/>
+        <font script="Mong" typeface="Mongolian Baiti"/>
+        <font script="Viet" typeface="Arial"/>
+        <font script="Uigh" typeface="Microsoft Uighur"/>
+        <font script="Geor" typeface="Sylfaen"/>
+      </minorFont>
+    </fontScheme>
+    <fmtScheme name="Office">
+      <fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9141,8 +9150,8 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
+      </fillStyleLst>
+      <lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -9164,8 +9173,8 @@
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
+      </lnStyleLst>
+      <effectStyleLst>
         <a:effectStyle>
           <a:effectLst/>
         </a:effectStyle>
@@ -9181,8 +9190,8 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
+      </effectStyleLst>
+      <bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9219,17 +9228,17 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
+      </bgFillStyleLst>
+    </fmtScheme>
+  </themeElements>
+  <objectDefaults/>
+  <extraClrSchemeLst/>
+  <extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
       <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
-  </a:extLst>
-</a:theme>
+  </extLst>
+</theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10729,7 +10738,7 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC9DF5F-13D1-4582-8C1D-D895F812E68F}">
   <sheetPr codeName="Sheet10">
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:BJ129"/>
   <sheetViews>
@@ -10737,10 +10746,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="12"/>
   <cols>
-    <col min="8" max="8" width="3.44140625" customWidth="1"/>
+    <col customWidth="true" max="8" min="8" width="3.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="3" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:62" s="3" customFormat="true" ht="18" customHeight="true">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -10748,7 +10757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:62" s="5" customFormat="1" ht="18" customHeight="1">
+    <row r="2" spans="1:62" s="5" customFormat="true" ht="18" customHeight="true">
       <c r="A2" s="32" t="s">
         <v>11</v>
       </c>
@@ -10820,7 +10829,7 @@
       <c r="BI2" s="27"/>
       <c r="BJ2" s="28"/>
     </row>
-    <row r="3" spans="1:62" s="3" customFormat="1" ht="18" customHeight="1">
+    <row r="3" spans="1:62" s="3" customFormat="true" ht="18" customHeight="true">
       <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
@@ -10892,7 +10901,7 @@
       <c r="BI3" s="27"/>
       <c r="BJ3" s="28"/>
     </row>
-    <row r="4" spans="1:62" s="3" customFormat="1" ht="18" customHeight="1">
+    <row r="4" spans="1:62" s="3" customFormat="true" ht="18" customHeight="true">
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
@@ -10958,9 +10967,9 @@
       <c r="BI4" s="27"/>
       <c r="BJ4" s="28"/>
     </row>
-    <row r="5" spans="1:62" s="1" customFormat="1" ht="4.5" customHeight="1"/>
-    <row r="6" spans="1:62" ht="11.25" customHeight="1"/>
-    <row r="7" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="5" spans="1:62" s="1" customFormat="true" ht="4.5" customHeight="true"/>
+    <row r="6" spans="1:62" ht="11.25" customHeight="true"/>
+    <row r="7" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A7" s="79" t="s">
         <v>12</v>
       </c>
@@ -11040,7 +11049,7 @@
       <c r="BI7" s="80"/>
       <c r="BJ7" s="81"/>
     </row>
-    <row r="8" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="8" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A8" s="48">
         <f t="shared" ref="A8:A88" si="0">ROW()-7</f>
         <v>1</v>
@@ -11113,7 +11122,7 @@
       <c r="BI8" s="125"/>
       <c r="BJ8" s="126"/>
     </row>
-    <row r="9" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="9" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A9" s="48">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -11186,7 +11195,7 @@
       <c r="BI9" s="125"/>
       <c r="BJ9" s="126"/>
     </row>
-    <row r="10" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="10" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A10" s="48">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -11261,7 +11270,7 @@
       <c r="BI10" s="125"/>
       <c r="BJ10" s="126"/>
     </row>
-    <row r="11" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="11" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A11" s="48">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -11336,7 +11345,7 @@
       <c r="BI11" s="125"/>
       <c r="BJ11" s="126"/>
     </row>
-    <row r="12" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="12" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A12" s="48">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -11411,7 +11420,7 @@
       <c r="BI12" s="125"/>
       <c r="BJ12" s="126"/>
     </row>
-    <row r="13" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="13" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A13" s="48">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -11484,7 +11493,7 @@
       <c r="BI13" s="125"/>
       <c r="BJ13" s="126"/>
     </row>
-    <row r="14" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="14" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A14" s="48">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -11557,7 +11566,7 @@
       <c r="BI14" s="125"/>
       <c r="BJ14" s="126"/>
     </row>
-    <row r="15" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="15" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A15" s="48">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -11630,7 +11639,7 @@
       <c r="BI15" s="125"/>
       <c r="BJ15" s="126"/>
     </row>
-    <row r="16" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="16" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A16" s="48">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -11703,7 +11712,7 @@
       <c r="BI16" s="125"/>
       <c r="BJ16" s="126"/>
     </row>
-    <row r="17" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="17" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A17" s="48">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -11776,7 +11785,7 @@
       <c r="BI17" s="125"/>
       <c r="BJ17" s="126"/>
     </row>
-    <row r="18" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="18" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A18" s="48">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -11849,7 +11858,7 @@
       <c r="BI18" s="125"/>
       <c r="BJ18" s="126"/>
     </row>
-    <row r="19" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="19" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A19" s="48">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -11922,7 +11931,7 @@
       <c r="BI19" s="125"/>
       <c r="BJ19" s="126"/>
     </row>
-    <row r="20" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="20" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A20" s="48">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -11995,7 +12004,7 @@
       <c r="BI20" s="125"/>
       <c r="BJ20" s="126"/>
     </row>
-    <row r="21" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="21" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A21" s="48">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -12068,7 +12077,7 @@
       <c r="BI21" s="125"/>
       <c r="BJ21" s="126"/>
     </row>
-    <row r="22" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="22" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A22" s="48">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -12143,7 +12152,7 @@
       <c r="BI22" s="125"/>
       <c r="BJ22" s="126"/>
     </row>
-    <row r="23" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="23" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A23" s="48">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -12218,7 +12227,7 @@
       <c r="BI23" s="125"/>
       <c r="BJ23" s="126"/>
     </row>
-    <row r="24" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="24" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A24" s="48">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -12232,7 +12241,7 @@
       <c r="F24" s="52"/>
       <c r="G24" s="52"/>
       <c r="H24" s="53"/>
-      <c r="I24" s="54" t="s">
+      <c r="I24" s="160" t="s">
         <v>1123</v>
       </c>
       <c r="J24" s="55"/>
@@ -12291,7 +12300,7 @@
       <c r="BI24" s="125"/>
       <c r="BJ24" s="126"/>
     </row>
-    <row r="25" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="25" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A25" s="48">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -12364,7 +12373,7 @@
       <c r="BI25" s="125"/>
       <c r="BJ25" s="126"/>
     </row>
-    <row r="26" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="26" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A26" s="48">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -12437,7 +12446,7 @@
       <c r="BI26" s="125"/>
       <c r="BJ26" s="126"/>
     </row>
-    <row r="27" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="27" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A27" s="48">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -12510,7 +12519,7 @@
       <c r="BI27" s="125"/>
       <c r="BJ27" s="126"/>
     </row>
-    <row r="28" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="28" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A28" s="48">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -12583,7 +12592,7 @@
       <c r="BI28" s="125"/>
       <c r="BJ28" s="126"/>
     </row>
-    <row r="29" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="29" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A29" s="48">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -12656,7 +12665,7 @@
       <c r="BI29" s="125"/>
       <c r="BJ29" s="126"/>
     </row>
-    <row r="30" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="30" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A30" s="48">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -12729,7 +12738,7 @@
       <c r="BI30" s="125"/>
       <c r="BJ30" s="126"/>
     </row>
-    <row r="31" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="31" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A31" s="48">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -12802,7 +12811,7 @@
       <c r="BI31" s="125"/>
       <c r="BJ31" s="126"/>
     </row>
-    <row r="32" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="32" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A32" s="48">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -12875,7 +12884,7 @@
       <c r="BI32" s="61"/>
       <c r="BJ32" s="62"/>
     </row>
-    <row r="33" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="33" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A33" s="48">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -12948,7 +12957,7 @@
       <c r="BI33" s="61"/>
       <c r="BJ33" s="62"/>
     </row>
-    <row r="34" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="34" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A34" s="48">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -13021,7 +13030,7 @@
       <c r="BI34" s="61"/>
       <c r="BJ34" s="62"/>
     </row>
-    <row r="35" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="35" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A35" s="48">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -13094,7 +13103,7 @@
       <c r="BI35" s="61"/>
       <c r="BJ35" s="62"/>
     </row>
-    <row r="36" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="36" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A36" s="48">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -13167,7 +13176,7 @@
       <c r="BI36" s="61"/>
       <c r="BJ36" s="62"/>
     </row>
-    <row r="37" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="37" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A37" s="48">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -13240,7 +13249,7 @@
       <c r="BI37" s="125"/>
       <c r="BJ37" s="126"/>
     </row>
-    <row r="38" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="38" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A38" s="48">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -13313,7 +13322,7 @@
       <c r="BI38" s="125"/>
       <c r="BJ38" s="126"/>
     </row>
-    <row r="39" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="39" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A39" s="48">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -13386,7 +13395,7 @@
       <c r="BI39" s="125"/>
       <c r="BJ39" s="126"/>
     </row>
-    <row r="40" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="40" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A40" s="48">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -13459,7 +13468,7 @@
       <c r="BI40" s="125"/>
       <c r="BJ40" s="126"/>
     </row>
-    <row r="41" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="41" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A41" s="48">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -13532,7 +13541,7 @@
       <c r="BI41" s="125"/>
       <c r="BJ41" s="126"/>
     </row>
-    <row r="42" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="42" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A42" s="48">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -13605,7 +13614,7 @@
       <c r="BI42" s="125"/>
       <c r="BJ42" s="126"/>
     </row>
-    <row r="43" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="43" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A43" s="48">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -13678,7 +13687,7 @@
       <c r="BI43" s="125"/>
       <c r="BJ43" s="126"/>
     </row>
-    <row r="44" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="44" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A44" s="48">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -13751,7 +13760,7 @@
       <c r="BI44" s="125"/>
       <c r="BJ44" s="126"/>
     </row>
-    <row r="45" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="45" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A45" s="48">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -13824,7 +13833,7 @@
       <c r="BI45" s="61"/>
       <c r="BJ45" s="62"/>
     </row>
-    <row r="46" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="46" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A46" s="48">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -13897,7 +13906,7 @@
       <c r="BI46" s="61"/>
       <c r="BJ46" s="62"/>
     </row>
-    <row r="47" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="47" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A47" s="48">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -13970,7 +13979,7 @@
       <c r="BI47" s="61"/>
       <c r="BJ47" s="62"/>
     </row>
-    <row r="48" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="48" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A48" s="48">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -14043,7 +14052,7 @@
       <c r="BI48" s="61"/>
       <c r="BJ48" s="62"/>
     </row>
-    <row r="49" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="49" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A49" s="48">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -14116,7 +14125,7 @@
       <c r="BI49" s="61"/>
       <c r="BJ49" s="62"/>
     </row>
-    <row r="50" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="50" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A50" s="48">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -14189,7 +14198,7 @@
       <c r="BI50" s="125"/>
       <c r="BJ50" s="126"/>
     </row>
-    <row r="51" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="51" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A51" s="48">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -14262,7 +14271,7 @@
       <c r="BI51" s="125"/>
       <c r="BJ51" s="126"/>
     </row>
-    <row r="52" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="52" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A52" s="48">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -14335,7 +14344,7 @@
       <c r="BI52" s="125"/>
       <c r="BJ52" s="126"/>
     </row>
-    <row r="53" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="53" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A53" s="48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -14408,7 +14417,7 @@
       <c r="BI53" s="125"/>
       <c r="BJ53" s="126"/>
     </row>
-    <row r="54" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="54" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A54" s="48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -14481,7 +14490,7 @@
       <c r="BI54" s="125"/>
       <c r="BJ54" s="126"/>
     </row>
-    <row r="55" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="55" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A55" s="48">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -14554,7 +14563,7 @@
       <c r="BI55" s="125"/>
       <c r="BJ55" s="126"/>
     </row>
-    <row r="56" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="56" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A56" s="48">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -14627,7 +14636,7 @@
       <c r="BI56" s="140"/>
       <c r="BJ56" s="141"/>
     </row>
-    <row r="57" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="57" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A57" s="48">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -14700,7 +14709,7 @@
       <c r="BI57" s="61"/>
       <c r="BJ57" s="62"/>
     </row>
-    <row r="58" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="58" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A58" s="48">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -14773,7 +14782,7 @@
       <c r="BI58" s="61"/>
       <c r="BJ58" s="62"/>
     </row>
-    <row r="59" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="59" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A59" s="48">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -14846,7 +14855,7 @@
       <c r="BI59" s="61"/>
       <c r="BJ59" s="62"/>
     </row>
-    <row r="60" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="60" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A60" s="48">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -14919,7 +14928,7 @@
       <c r="BI60" s="61"/>
       <c r="BJ60" s="62"/>
     </row>
-    <row r="61" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="61" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A61" s="48">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -14992,7 +15001,7 @@
       <c r="BI61" s="125"/>
       <c r="BJ61" s="126"/>
     </row>
-    <row r="62" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="62" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A62" s="48">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -15065,7 +15074,7 @@
       <c r="BI62" s="125"/>
       <c r="BJ62" s="126"/>
     </row>
-    <row r="63" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="63" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A63" s="48">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -15138,7 +15147,7 @@
       <c r="BI63" s="125"/>
       <c r="BJ63" s="126"/>
     </row>
-    <row r="64" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="64" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A64" s="48">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -15211,7 +15220,7 @@
       <c r="BI64" s="125"/>
       <c r="BJ64" s="126"/>
     </row>
-    <row r="65" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="65" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A65" s="48">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -15284,7 +15293,7 @@
       <c r="BI65" s="125"/>
       <c r="BJ65" s="126"/>
     </row>
-    <row r="66" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="66" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A66" s="48">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -15357,7 +15366,7 @@
       <c r="BI66" s="125"/>
       <c r="BJ66" s="126"/>
     </row>
-    <row r="67" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="67" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A67" s="48">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -15430,7 +15439,7 @@
       <c r="BI67" s="125"/>
       <c r="BJ67" s="126"/>
     </row>
-    <row r="68" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="68" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A68" s="48">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -15503,7 +15512,7 @@
       <c r="BI68" s="125"/>
       <c r="BJ68" s="126"/>
     </row>
-    <row r="69" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="69" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A69" s="48">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -15576,7 +15585,7 @@
       <c r="BI69" s="125"/>
       <c r="BJ69" s="126"/>
     </row>
-    <row r="70" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="70" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A70" s="48">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -15649,7 +15658,7 @@
       <c r="BI70" s="61"/>
       <c r="BJ70" s="62"/>
     </row>
-    <row r="71" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="71" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A71" s="48">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -15722,7 +15731,7 @@
       <c r="BI71" s="125"/>
       <c r="BJ71" s="126"/>
     </row>
-    <row r="72" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="72" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A72" s="48">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -15795,7 +15804,7 @@
       <c r="BI72" s="125"/>
       <c r="BJ72" s="126"/>
     </row>
-    <row r="73" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="73" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A73" s="48">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -15868,7 +15877,7 @@
       <c r="BI73" s="125"/>
       <c r="BJ73" s="126"/>
     </row>
-    <row r="74" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="74" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A74" s="48">
         <f t="shared" si="0"/>
         <v>67</v>
@@ -15941,7 +15950,7 @@
       <c r="BI74" s="125"/>
       <c r="BJ74" s="126"/>
     </row>
-    <row r="75" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="75" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A75" s="48">
         <f t="shared" si="0"/>
         <v>68</v>
@@ -16016,7 +16025,7 @@
       <c r="BI75" s="125"/>
       <c r="BJ75" s="126"/>
     </row>
-    <row r="76" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="76" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A76" s="48">
         <f t="shared" si="0"/>
         <v>69</v>
@@ -16091,7 +16100,7 @@
       <c r="BI76" s="125"/>
       <c r="BJ76" s="126"/>
     </row>
-    <row r="77" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="77" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A77" s="48">
         <f t="shared" si="0"/>
         <v>70</v>
@@ -16164,7 +16173,7 @@
       <c r="BI77" s="125"/>
       <c r="BJ77" s="126"/>
     </row>
-    <row r="78" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="78" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A78" s="48">
         <f t="shared" si="0"/>
         <v>71</v>
@@ -16239,7 +16248,7 @@
       <c r="BI78" s="125"/>
       <c r="BJ78" s="126"/>
     </row>
-    <row r="79" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="79" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A79" s="48">
         <f t="shared" si="0"/>
         <v>72</v>
@@ -16314,7 +16323,7 @@
       <c r="BI79" s="125"/>
       <c r="BJ79" s="126"/>
     </row>
-    <row r="80" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="80" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A80" s="48">
         <f t="shared" si="0"/>
         <v>73</v>
@@ -16389,7 +16398,7 @@
       <c r="BI80" s="125"/>
       <c r="BJ80" s="126"/>
     </row>
-    <row r="81" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="81" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A81" s="48">
         <f t="shared" si="0"/>
         <v>74</v>
@@ -16464,7 +16473,7 @@
       <c r="BI81" s="125"/>
       <c r="BJ81" s="126"/>
     </row>
-    <row r="82" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="82" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A82" s="48">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -16539,7 +16548,7 @@
       <c r="BI82" s="125"/>
       <c r="BJ82" s="126"/>
     </row>
-    <row r="83" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="83" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A83" s="48">
         <f t="shared" si="0"/>
         <v>76</v>
@@ -16614,7 +16623,7 @@
       <c r="BI83" s="125"/>
       <c r="BJ83" s="126"/>
     </row>
-    <row r="84" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="84" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A84" s="48">
         <f t="shared" si="0"/>
         <v>77</v>
@@ -16689,7 +16698,7 @@
       <c r="BI84" s="125"/>
       <c r="BJ84" s="126"/>
     </row>
-    <row r="85" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="85" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A85" s="48">
         <f t="shared" si="0"/>
         <v>78</v>
@@ -16762,7 +16771,7 @@
       <c r="BI85" s="125"/>
       <c r="BJ85" s="126"/>
     </row>
-    <row r="86" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="86" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A86" s="48">
         <f t="shared" si="0"/>
         <v>79</v>
@@ -16835,7 +16844,7 @@
       <c r="BI86" s="125"/>
       <c r="BJ86" s="126"/>
     </row>
-    <row r="87" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="87" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A87" s="48">
         <f t="shared" si="0"/>
         <v>80</v>
@@ -16908,7 +16917,7 @@
       <c r="BI87" s="125"/>
       <c r="BJ87" s="126"/>
     </row>
-    <row r="88" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="88" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A88" s="48">
         <f t="shared" si="0"/>
         <v>81</v>
@@ -16981,7 +16990,7 @@
       <c r="BI88" s="125"/>
       <c r="BJ88" s="126"/>
     </row>
-    <row r="89" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="89" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A89" s="48"/>
       <c r="B89" s="49"/>
       <c r="C89" s="50"/>
@@ -17053,7 +17062,7 @@
       <c r="BI89" s="125"/>
       <c r="BJ89" s="126"/>
     </row>
-    <row r="90" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="90" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A90" s="48"/>
       <c r="B90" s="49"/>
       <c r="C90" s="50"/>
@@ -17117,7 +17126,7 @@
       <c r="BI90" s="61"/>
       <c r="BJ90" s="62"/>
     </row>
-    <row r="91" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="91" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A91" s="48"/>
       <c r="B91" s="49"/>
       <c r="C91" s="50"/>
@@ -17181,7 +17190,7 @@
       <c r="BI91" s="61"/>
       <c r="BJ91" s="62"/>
     </row>
-    <row r="92" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="92" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A92" s="48"/>
       <c r="B92" s="49"/>
       <c r="C92" s="50"/>
@@ -17245,7 +17254,7 @@
       <c r="BI92" s="61"/>
       <c r="BJ92" s="62"/>
     </row>
-    <row r="93" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="93" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A93" s="48"/>
       <c r="B93" s="49"/>
       <c r="C93" s="50"/>
@@ -17309,7 +17318,7 @@
       <c r="BI93" s="61"/>
       <c r="BJ93" s="62"/>
     </row>
-    <row r="94" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="94" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A94" s="48"/>
       <c r="B94" s="49"/>
       <c r="C94" s="50"/>
@@ -17373,7 +17382,7 @@
       <c r="BI94" s="61"/>
       <c r="BJ94" s="62"/>
     </row>
-    <row r="95" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="95" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A95" s="48"/>
       <c r="B95" s="49"/>
       <c r="C95" s="50"/>
@@ -17437,7 +17446,7 @@
       <c r="BI95" s="61"/>
       <c r="BJ95" s="62"/>
     </row>
-    <row r="96" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="96" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A96" s="48"/>
       <c r="B96" s="49"/>
       <c r="C96" s="50"/>
@@ -17501,7 +17510,7 @@
       <c r="BI96" s="61"/>
       <c r="BJ96" s="62"/>
     </row>
-    <row r="97" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="97" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A97" s="48"/>
       <c r="B97" s="49"/>
       <c r="C97" s="50"/>
@@ -17565,7 +17574,7 @@
       <c r="BI97" s="61"/>
       <c r="BJ97" s="62"/>
     </row>
-    <row r="98" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="98" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A98" s="48"/>
       <c r="B98" s="49"/>
       <c r="C98" s="50"/>
@@ -17629,7 +17638,7 @@
       <c r="BI98" s="61"/>
       <c r="BJ98" s="62"/>
     </row>
-    <row r="99" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="99" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A99" s="48"/>
       <c r="B99" s="49"/>
       <c r="C99" s="50"/>
@@ -17693,7 +17702,7 @@
       <c r="BI99" s="61"/>
       <c r="BJ99" s="62"/>
     </row>
-    <row r="100" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="100" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A100" s="48"/>
       <c r="B100" s="49"/>
       <c r="C100" s="50"/>
@@ -17757,7 +17766,7 @@
       <c r="BI100" s="61"/>
       <c r="BJ100" s="62"/>
     </row>
-    <row r="101" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="101" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A101" s="48"/>
       <c r="B101" s="49"/>
       <c r="C101" s="50"/>
@@ -17821,7 +17830,7 @@
       <c r="BI101" s="61"/>
       <c r="BJ101" s="62"/>
     </row>
-    <row r="102" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="102" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A102" s="48"/>
       <c r="B102" s="49"/>
       <c r="C102" s="50"/>
@@ -17885,7 +17894,7 @@
       <c r="BI102" s="61"/>
       <c r="BJ102" s="62"/>
     </row>
-    <row r="103" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="103" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A103" s="48"/>
       <c r="B103" s="49"/>
       <c r="C103" s="50"/>
@@ -17949,7 +17958,7 @@
       <c r="BI103" s="61"/>
       <c r="BJ103" s="62"/>
     </row>
-    <row r="104" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="104" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A104" s="48"/>
       <c r="B104" s="49"/>
       <c r="C104" s="50"/>
@@ -18013,7 +18022,7 @@
       <c r="BI104" s="61"/>
       <c r="BJ104" s="62"/>
     </row>
-    <row r="105" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="105" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A105" s="48"/>
       <c r="B105" s="49"/>
       <c r="C105" s="50"/>
@@ -18077,7 +18086,7 @@
       <c r="BI105" s="61"/>
       <c r="BJ105" s="62"/>
     </row>
-    <row r="106" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="106" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A106" s="48"/>
       <c r="B106" s="49"/>
       <c r="C106" s="50"/>
@@ -18141,7 +18150,7 @@
       <c r="BI106" s="61"/>
       <c r="BJ106" s="62"/>
     </row>
-    <row r="107" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="107" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A107" s="48"/>
       <c r="B107" s="49"/>
       <c r="C107" s="50"/>
@@ -18205,7 +18214,7 @@
       <c r="BI107" s="61"/>
       <c r="BJ107" s="62"/>
     </row>
-    <row r="108" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="108" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A108" s="48"/>
       <c r="B108" s="49"/>
       <c r="C108" s="50"/>
@@ -18269,7 +18278,7 @@
       <c r="BI108" s="61"/>
       <c r="BJ108" s="62"/>
     </row>
-    <row r="109" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="109" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A109" s="48"/>
       <c r="B109" s="49"/>
       <c r="C109" s="50"/>
@@ -18333,7 +18342,7 @@
       <c r="BI109" s="61"/>
       <c r="BJ109" s="62"/>
     </row>
-    <row r="110" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="110" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A110" s="48"/>
       <c r="B110" s="49"/>
       <c r="C110" s="50"/>
@@ -18397,7 +18406,7 @@
       <c r="BI110" s="61"/>
       <c r="BJ110" s="62"/>
     </row>
-    <row r="111" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="111" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A111" s="48"/>
       <c r="B111" s="49"/>
       <c r="C111" s="50"/>
@@ -18461,7 +18470,7 @@
       <c r="BI111" s="61"/>
       <c r="BJ111" s="62"/>
     </row>
-    <row r="112" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="112" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A112" s="48"/>
       <c r="B112" s="49"/>
       <c r="C112" s="50"/>
@@ -18525,7 +18534,7 @@
       <c r="BI112" s="61"/>
       <c r="BJ112" s="62"/>
     </row>
-    <row r="113" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="113" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A113" s="48"/>
       <c r="B113" s="49"/>
       <c r="C113" s="50"/>
@@ -18589,7 +18598,7 @@
       <c r="BI113" s="61"/>
       <c r="BJ113" s="62"/>
     </row>
-    <row r="114" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="114" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A114" s="48"/>
       <c r="B114" s="49"/>
       <c r="C114" s="50"/>
@@ -18653,7 +18662,7 @@
       <c r="BI114" s="61"/>
       <c r="BJ114" s="62"/>
     </row>
-    <row r="115" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="115" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A115" s="48"/>
       <c r="B115" s="49"/>
       <c r="C115" s="50"/>
@@ -18717,7 +18726,7 @@
       <c r="BI115" s="61"/>
       <c r="BJ115" s="62"/>
     </row>
-    <row r="116" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="116" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A116" s="48"/>
       <c r="B116" s="49"/>
       <c r="C116" s="50"/>
@@ -18781,7 +18790,7 @@
       <c r="BI116" s="61"/>
       <c r="BJ116" s="62"/>
     </row>
-    <row r="117" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="117" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A117" s="48"/>
       <c r="B117" s="49"/>
       <c r="C117" s="50"/>
@@ -18845,7 +18854,7 @@
       <c r="BI117" s="61"/>
       <c r="BJ117" s="62"/>
     </row>
-    <row r="118" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="118" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A118" s="48"/>
       <c r="B118" s="49"/>
       <c r="C118" s="50"/>
@@ -18909,7 +18918,7 @@
       <c r="BI118" s="61"/>
       <c r="BJ118" s="62"/>
     </row>
-    <row r="119" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="119" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A119" s="48"/>
       <c r="B119" s="49"/>
       <c r="C119" s="50"/>
@@ -18973,7 +18982,7 @@
       <c r="BI119" s="61"/>
       <c r="BJ119" s="62"/>
     </row>
-    <row r="120" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="120" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A120" s="48"/>
       <c r="B120" s="49"/>
       <c r="C120" s="50"/>
@@ -19037,7 +19046,7 @@
       <c r="BI120" s="61"/>
       <c r="BJ120" s="62"/>
     </row>
-    <row r="121" spans="1:62" s="16" customFormat="1" ht="30.75" customHeight="1">
+    <row r="121" spans="1:62" s="16" customFormat="true" ht="30.75" customHeight="true">
       <c r="A121" s="88"/>
       <c r="B121" s="89"/>
       <c r="C121" s="90"/>
@@ -19101,70 +19110,70 @@
       <c r="BI121" s="101"/>
       <c r="BJ121" s="102"/>
     </row>
-    <row r="122" spans="1:62" s="2" customFormat="1" ht="6" customHeight="1"/>
-    <row r="123" spans="1:62" s="2" customFormat="1" ht="13.5" customHeight="1"/>
-    <row r="124" spans="1:62" ht="18" customHeight="1"/>
-    <row r="125" spans="1:62" ht="18" customHeight="1"/>
-    <row r="126" spans="1:62" ht="18" customHeight="1"/>
-    <row r="127" spans="1:62" ht="18" customHeight="1"/>
-    <row r="128" spans="1:62" ht="18" customHeight="1"/>
-    <row r="129" ht="18" customHeight="1"/>
+    <row r="122" spans="1:62" s="2" customFormat="true" ht="6" customHeight="true"/>
+    <row r="123" spans="1:62" s="2" customFormat="true" ht="13.5" customHeight="true"/>
+    <row r="124" spans="1:62" ht="18" customHeight="true"/>
+    <row r="125" spans="1:62" ht="18" customHeight="true"/>
+    <row r="126" spans="1:62" ht="18" customHeight="true"/>
+    <row r="127" spans="1:62" ht="18" customHeight="true"/>
+    <row r="128" spans="1:62" ht="18" customHeight="true"/>
+    <row r="129" ht="18" customHeight="true"/>
   </sheetData>
-  <autoFilter ref="A7:BJ88" xr:uid="{DFC9DF5F-13D1-4582-8C1D-D895F812E68F}">
-    <filterColumn colId="0" showButton="0"/>
-    <filterColumn colId="1" showButton="0"/>
-    <filterColumn colId="3" showButton="0"/>
-    <filterColumn colId="4" showButton="0"/>
-    <filterColumn colId="5" showButton="0"/>
-    <filterColumn colId="6" showButton="0"/>
-    <filterColumn colId="8" showButton="0"/>
-    <filterColumn colId="9" showButton="0"/>
-    <filterColumn colId="10" showButton="0"/>
-    <filterColumn colId="11" showButton="0"/>
-    <filterColumn colId="12" showButton="0"/>
-    <filterColumn colId="13" showButton="0"/>
-    <filterColumn colId="14" showButton="0"/>
-    <filterColumn colId="15" showButton="0"/>
-    <filterColumn colId="16" showButton="0"/>
-    <filterColumn colId="17" showButton="0"/>
-    <filterColumn colId="18" showButton="0"/>
-    <filterColumn colId="19" showButton="0"/>
-    <filterColumn colId="20" showButton="0"/>
-    <filterColumn colId="21" showButton="0"/>
-    <filterColumn colId="22" showButton="0"/>
-    <filterColumn colId="23" showButton="0"/>
-    <filterColumn colId="24" showButton="0"/>
-    <filterColumn colId="25" showButton="0"/>
-    <filterColumn colId="26" showButton="0"/>
-    <filterColumn colId="27" showButton="0"/>
-    <filterColumn colId="28" showButton="0"/>
-    <filterColumn colId="29" showButton="0"/>
-    <filterColumn colId="30" showButton="0"/>
-    <filterColumn colId="31" showButton="0"/>
-    <filterColumn colId="32" showButton="0"/>
-    <filterColumn colId="34" showButton="0"/>
-    <filterColumn colId="35" showButton="0"/>
-    <filterColumn colId="37" showButton="0"/>
-    <filterColumn colId="38" showButton="0"/>
-    <filterColumn colId="40" showButton="0"/>
-    <filterColumn colId="41" showButton="0"/>
-    <filterColumn colId="43" showButton="0"/>
-    <filterColumn colId="44" showButton="0"/>
-    <filterColumn colId="46" showButton="0"/>
-    <filterColumn colId="47" showButton="0"/>
-    <filterColumn colId="48" showButton="0"/>
-    <filterColumn colId="49" showButton="0"/>
-    <filterColumn colId="50" showButton="0"/>
-    <filterColumn colId="51" showButton="0"/>
-    <filterColumn colId="52" showButton="0"/>
-    <filterColumn colId="53" showButton="0"/>
-    <filterColumn colId="54" showButton="0"/>
-    <filterColumn colId="55" showButton="0"/>
-    <filterColumn colId="56" showButton="0"/>
-    <filterColumn colId="57" showButton="0"/>
-    <filterColumn colId="58" showButton="0"/>
-    <filterColumn colId="59" showButton="0"/>
-    <filterColumn colId="60" showButton="0"/>
+  <autoFilter ref="A7:BJ88">
+    <filterColumn colId="0"/>
+    <filterColumn colId="1"/>
+    <filterColumn colId="3"/>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
+    <filterColumn colId="6"/>
+    <filterColumn colId="8"/>
+    <filterColumn colId="9"/>
+    <filterColumn colId="10"/>
+    <filterColumn colId="11"/>
+    <filterColumn colId="12"/>
+    <filterColumn colId="13"/>
+    <filterColumn colId="14"/>
+    <filterColumn colId="15"/>
+    <filterColumn colId="16"/>
+    <filterColumn colId="17"/>
+    <filterColumn colId="18"/>
+    <filterColumn colId="19"/>
+    <filterColumn colId="20"/>
+    <filterColumn colId="21"/>
+    <filterColumn colId="22"/>
+    <filterColumn colId="23"/>
+    <filterColumn colId="24"/>
+    <filterColumn colId="25"/>
+    <filterColumn colId="26"/>
+    <filterColumn colId="27"/>
+    <filterColumn colId="28"/>
+    <filterColumn colId="29"/>
+    <filterColumn colId="30"/>
+    <filterColumn colId="31"/>
+    <filterColumn colId="32"/>
+    <filterColumn colId="34"/>
+    <filterColumn colId="35"/>
+    <filterColumn colId="37"/>
+    <filterColumn colId="38"/>
+    <filterColumn colId="40"/>
+    <filterColumn colId="41"/>
+    <filterColumn colId="43"/>
+    <filterColumn colId="44"/>
+    <filterColumn colId="46"/>
+    <filterColumn colId="47"/>
+    <filterColumn colId="48"/>
+    <filterColumn colId="49"/>
+    <filterColumn colId="50"/>
+    <filterColumn colId="51"/>
+    <filterColumn colId="52"/>
+    <filterColumn colId="53"/>
+    <filterColumn colId="54"/>
+    <filterColumn colId="55"/>
+    <filterColumn colId="56"/>
+    <filterColumn colId="57"/>
+    <filterColumn colId="58"/>
+    <filterColumn colId="59"/>
+    <filterColumn colId="60"/>
   </autoFilter>
   <mergeCells count="931">
     <mergeCell ref="A81:C81"/>
@@ -20100,10 +20109,10 @@
     <mergeCell ref="A105:C105"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.15748031496062992" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7086614173228347" right="0.7086614173228347" top="0.15748031496062992" bottom="0.7480314960629921" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup fitToHeight="0" r:id="rId1" orientation="portrait" paperSize="9" scale="63"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;R&amp;P   </oddHeader>
+    <oddHeader>&amp;R&amp;P   </oddHeader>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>